<commit_message>
simple model for testing
</commit_message>
<xml_diff>
--- a/Phase2-answer/Pahse2_Data_OR2.xlsx
+++ b/Phase2-answer/Pahse2_Data_OR2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University\Terme 7\TA\OR2\Phase 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase2-answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3699803-A92C-496C-8670-BA26979C77CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3035E279-7F74-43C9-9E4C-ED341A7A15BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
   </bookViews>
   <sheets>
     <sheet name="D" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Unskilled</t>
   </si>
@@ -40,18 +40,6 @@
     <t>Skilled</t>
   </si>
   <si>
-    <t>Current strength</t>
-  </si>
-  <si>
-    <t>Year 1</t>
-  </si>
-  <si>
-    <t>Year 2</t>
-  </si>
-  <si>
-    <t>Year 3</t>
-  </si>
-  <si>
     <t>Less than one year's service</t>
   </si>
   <si>
@@ -74,6 +62,9 @@
   </si>
   <si>
     <t>Cost of short-time working per employee per year</t>
+  </si>
+  <si>
+    <t>year\skill</t>
   </si>
 </sst>
 </file>
@@ -105,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE8D9F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,12 +219,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -253,6 +244,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,30 +572,28 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,9 +604,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <v>2000</v>
@@ -626,9 +618,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>1000</v>
@@ -640,9 +632,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>500</v>
@@ -654,9 +646,9 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>6</v>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -678,66 +670,62 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8">
-        <v>25</v>
-      </c>
-      <c r="D3" s="8">
-        <v>20</v>
-      </c>
-      <c r="E3" s="8">
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8">
-        <v>10</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
     </row>
@@ -751,51 +739,47 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="39.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8">
         <v>500</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>800</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>500</v>
       </c>
     </row>
@@ -809,49 +793,45 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="11" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="12">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10">
         <v>1500</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>2000</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>3000</v>
       </c>
     </row>
@@ -865,49 +845,45 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="14">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12">
         <v>500</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>400</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds hire constraint and param indice
</commit_message>
<xml_diff>
--- a/Phase2-answer/Pahse2_Data_OR2.xlsx
+++ b/Phase2-answer/Pahse2_Data_OR2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase2-answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816D6FD-AF5E-4F7C-8327-9770EC0D75AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494B28A-A6E8-4DFE-853B-FDFE0E61C9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="4275" windowWidth="21600" windowHeight="11325" activeTab="6" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Unskilled</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -826,10 +829,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="D5:E6"/>
+  <dimension ref="D4:E8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,9 +840,14 @@
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D5" s="14" t="s">
         <v>7</v>
@@ -848,11 +856,16 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="14" t="s">
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E8" s="15">
         <v>0.25</v>
       </c>
     </row>
@@ -869,7 +882,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +921,11 @@
         <v>3000</v>
       </c>
     </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>9</v>
@@ -926,10 +944,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,10 +987,15 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C6" s="12">
         <v>50</v>
       </c>
     </row>
@@ -986,7 +1009,7 @@
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding cost to excel
</commit_message>
<xml_diff>
--- a/Phase2-answer/Pahse2_Data_OR2.xlsx
+++ b/Phase2-answer/Pahse2_Data_OR2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase2-answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33141E5A-B6BB-42D9-8F88-67BDFE2AD676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EB13D0-7FFA-40C3-85E4-DDF64C4E0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="7" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
   </bookViews>
   <sheets>
     <sheet name="D" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
   <si>
     <t>Unskilled</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>Layoff Cost</t>
+  </si>
+  <si>
+    <t>Training Cost</t>
+  </si>
+  <si>
+    <t>Parttime Cost</t>
+  </si>
+  <si>
+    <t>Overhire Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
   <si>
     <t>Eps</t>
@@ -341,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +423,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1187,9 +1202,9 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:H62"/>
+  <dimension ref="B1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1285,10 +1300,10 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1313,7 +1328,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>800</v>
@@ -1327,13 +1342,13 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -1352,13 +1367,13 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -1366,13 +1381,13 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -1380,13 +1395,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -1394,13 +1409,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -1419,13 +1434,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -1433,13 +1448,13 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -1447,13 +1462,13 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -1461,13 +1476,13 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -1489,10 +1504,10 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
@@ -1500,10 +1515,10 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E28">
         <v>100</v>
@@ -1517,7 +1532,7 @@
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E29">
         <v>140</v>
@@ -1528,13 +1543,13 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
@@ -1556,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E33">
         <v>200</v>
@@ -1570,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F34">
         <v>41</v>
@@ -1584,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
@@ -1595,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E36">
         <v>200</v>
@@ -1609,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F37">
         <v>10</v>
@@ -1625,7 +1640,7 @@
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
@@ -1636,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
@@ -1648,7 +1663,7 @@
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F40" s="16"/>
     </row>
@@ -1660,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
@@ -1671,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
@@ -1682,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
@@ -1693,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
@@ -1737,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
@@ -1751,7 +1766,7 @@
         <v>184</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
@@ -1762,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
@@ -1773,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
@@ -1784,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
@@ -1795,7 +1810,7 @@
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
@@ -1806,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
@@ -1828,7 +1843,7 @@
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
@@ -1839,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
@@ -1850,7 +1865,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
@@ -1861,7 +1876,22 @@
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>738000</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>738400</v>
       </c>
     </row>
   </sheetData>
@@ -1876,8 +1906,8 @@
   </sheetPr>
   <dimension ref="A2:T74"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="108" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3038,6 +3068,22 @@
         <f>IF(Results!E24= "Eps", 0, Results!E24)</f>
         <v>0</v>
       </c>
+      <c r="G24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="21">
+        <f>Results!B65</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G25" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="21">
+        <f>Results!B67</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
@@ -3055,6 +3101,13 @@
         <f>IF(Results!E26= "Eps", 0, Results!E26)</f>
         <v>Skilled</v>
       </c>
+      <c r="G26" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="21">
+        <f>Results!B69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
@@ -3075,6 +3128,13 @@
       <c r="E27" s="17">
         <f>IF(Results!E27= "Eps", 0, Results!E27)</f>
         <v>0</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="21">
+        <f>Results!B71</f>
+        <v>738000</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -3094,6 +3154,13 @@
       <c r="E28" s="17">
         <f>IF(Results!E28= "Eps", 0, Results!E28)</f>
         <v>100</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="21">
+        <f>Results!B73</f>
+        <v>738400</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
remove given demand equation
</commit_message>
<xml_diff>
--- a/Phase2-answer/Pahse2_Data_OR2.xlsx
+++ b/Phase2-answer/Pahse2_Data_OR2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase2-answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EB13D0-7FFA-40C3-85E4-DDF64C4E0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC578ACC-ED5C-414A-AEAF-0DBD3CE1D537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="44">
   <si>
     <t>Unskilled</t>
   </si>
@@ -972,26 +972,27 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="D4:E8"/>
+  <dimension ref="C4:G15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
@@ -999,18 +1000,63 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="15">
         <v>0.25</v>
       </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15">
+        <v>400</v>
+      </c>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1025,7 +1071,7 @@
   <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,7 +1293,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>1695</v>
+        <v>1000</v>
       </c>
       <c r="D4">
         <v>1400</v>
@@ -1261,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>1360</v>
+        <v>500</v>
       </c>
       <c r="D5">
         <v>2000</v>
@@ -1274,14 +1320,14 @@
       <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
-        <v>1230</v>
+      <c r="C6" t="s">
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>2540</v>
+        <v>2500</v>
       </c>
       <c r="E6">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -1306,18 +1352,18 @@
         <v>43</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>60.000000183920243</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
-        <v>46</v>
+      <c r="C10" t="s">
+        <v>43</v>
       </c>
       <c r="D10">
-        <v>600.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -1334,7 +1380,7 @@
         <v>800</v>
       </c>
       <c r="E11">
-        <v>500.0000000000004</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -1433,8 +1479,8 @@
       <c r="B21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>43</v>
+      <c r="C21">
+        <v>814.0000000413819</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
@@ -1447,8 +1493,8 @@
       <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
-        <v>43</v>
+      <c r="C22">
+        <v>269.99999999999983</v>
       </c>
       <c r="D22" t="s">
         <v>43</v>
@@ -1461,8 +1507,8 @@
       <c r="B23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C23" t="s">
-        <v>43</v>
+      <c r="C23">
+        <v>364.99999999999966</v>
       </c>
       <c r="D23" t="s">
         <v>43</v>
@@ -1500,8 +1546,8 @@
       <c r="B27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C27">
-        <v>4</v>
+      <c r="C27" t="s">
+        <v>43</v>
       </c>
       <c r="D27" t="s">
         <v>43</v>
@@ -1520,22 +1566,22 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28">
-        <v>100</v>
+      <c r="E28" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C29">
-        <v>8</v>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>43</v>
       </c>
-      <c r="E29">
-        <v>140</v>
+      <c r="E29" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
@@ -1573,9 +1619,6 @@
       <c r="D33" t="s">
         <v>43</v>
       </c>
-      <c r="E33">
-        <v>200</v>
-      </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
@@ -1587,9 +1630,6 @@
       <c r="E34" t="s">
         <v>43</v>
       </c>
-      <c r="F34">
-        <v>41</v>
-      </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
@@ -1613,7 +1653,7 @@
         <v>43</v>
       </c>
       <c r="E36">
-        <v>200</v>
+        <v>130.00000000000017</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
@@ -1627,7 +1667,7 @@
         <v>43</v>
       </c>
       <c r="F37">
-        <v>10</v>
+        <v>100.00000000000018</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
@@ -1653,6 +1693,9 @@
       <c r="D39" t="s">
         <v>43</v>
       </c>
+      <c r="E39">
+        <v>85.000000000000369</v>
+      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
@@ -1665,7 +1708,9 @@
       <c r="E40" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="16"/>
+      <c r="F40" s="16">
+        <v>125</v>
+      </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
@@ -1763,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>184</v>
+        <v>26.000000082763837</v>
       </c>
       <c r="E52" t="s">
         <v>43</v>
@@ -1776,6 +1821,12 @@
       <c r="C53" s="16" t="s">
         <v>2</v>
       </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>2.0000001655280357</v>
+      </c>
       <c r="F53" t="s">
         <v>43</v>
       </c>
@@ -1881,17 +1932,17 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B71">
-        <v>738000</v>
+        <v>198500.00000000029</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>289800.00000827626</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73">
-        <v>738400</v>
+        <v>488300.00000827655</v>
       </c>
     </row>
   </sheetData>
@@ -1906,8 +1957,8 @@
   </sheetPr>
   <dimension ref="A2:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="108" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2020,7 +2071,7 @@
       </c>
       <c r="C4" s="17">
         <f>IF(Results!C4= "Eps", 0, Results!C4)</f>
-        <v>1695</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="17">
         <f>IF(Results!D4= "Eps", 0, Results!D4)</f>
@@ -2047,23 +2098,23 @@
       </c>
       <c r="K4" s="17">
         <f>VLOOKUP($G4,$B$21:$E$24,2,FALSE)</f>
-        <v>0</v>
+        <v>814.0000000413819</v>
       </c>
       <c r="L4" s="23">
         <f>VLOOKUP($G4,$B$27:$E$30,2,FALSE)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M4" s="17">
         <f>E33</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N4" s="17">
         <f>D49</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4" s="17">
         <f>D48</f>
-        <v>184</v>
+        <v>26.000000082763837</v>
       </c>
       <c r="P4" s="23">
         <v>0</v>
@@ -2088,7 +2139,7 @@
       </c>
       <c r="C5" s="17">
         <f>IF(Results!C5= "Eps", 0, Results!C5)</f>
-        <v>1360</v>
+        <v>500</v>
       </c>
       <c r="D5" s="17">
         <f>IF(Results!D5= "Eps", 0, Results!D5)</f>
@@ -2103,11 +2154,11 @@
       </c>
       <c r="H5" s="23">
         <f>VLOOKUP($G5,$B$3:$E$6,2,FALSE)</f>
-        <v>1695</v>
+        <v>1000</v>
       </c>
       <c r="I5" s="17">
         <f>VLOOKUP($G5,$B$9:$E$12,2,FALSE)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J5" s="17">
         <f>VLOOKUP($G5,$B$15:$E$18,2,FALSE)</f>
@@ -2115,7 +2166,7 @@
       </c>
       <c r="K5" s="17">
         <f>VLOOKUP($G5,$B$21:$E$24,2,FALSE)</f>
-        <v>0</v>
+        <v>269.99999999999983</v>
       </c>
       <c r="L5" s="23">
         <f>VLOOKUP($G5,$B$27:$E$30,2,FALSE)</f>
@@ -2123,7 +2174,7 @@
       </c>
       <c r="M5" s="17">
         <f>E36</f>
-        <v>200</v>
+        <v>130.00000000000017</v>
       </c>
       <c r="N5" s="17">
         <f>D52</f>
@@ -2135,7 +2186,7 @@
       </c>
       <c r="P5" s="23">
         <f>$B$67/100* (I4+ L4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="23">
         <f>0.01* $B$68* (H4)</f>
@@ -2143,7 +2194,7 @@
       </c>
       <c r="R5" s="23">
         <f>R4+I4+L4-K4-M4+0.5* N4+0.5* O4-P5-Q5</f>
-        <v>1695</v>
+        <v>1000</v>
       </c>
       <c r="S5" s="17">
         <f>B72</f>
@@ -2158,22 +2209,22 @@
       </c>
       <c r="C6" s="17">
         <f>IF(Results!C6= "Eps", 0, Results!C6)</f>
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="D6" s="17">
         <f>IF(Results!D6= "Eps", 0, Results!D6)</f>
-        <v>2540</v>
+        <v>2500</v>
       </c>
       <c r="E6" s="17">
         <f>IF(Results!E6= "Eps", 0, Results!E6)</f>
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G6" s="19">
         <v>2</v>
       </c>
       <c r="H6" s="23">
         <f>VLOOKUP($G6,$B$3:$E$6,2,FALSE)</f>
-        <v>1360</v>
+        <v>500</v>
       </c>
       <c r="I6" s="17">
         <f>VLOOKUP($G6,$B$9:$E$12,2,FALSE)</f>
@@ -2185,15 +2236,15 @@
       </c>
       <c r="K6" s="17">
         <f>VLOOKUP($G6,$B$21:$E$24,2,FALSE)</f>
-        <v>0</v>
+        <v>364.99999999999966</v>
       </c>
       <c r="L6" s="23">
         <f>VLOOKUP($G6,$B$27:$E$30,2,FALSE)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M6" s="17">
         <f>E39</f>
-        <v>0</v>
+        <v>85.000000000000369</v>
       </c>
       <c r="N6" s="17">
         <f>D55</f>
@@ -2205,15 +2256,15 @@
       </c>
       <c r="P6" s="23">
         <f>$B$67/100* (I5+ L5)</f>
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="23">
         <f>0.01* $B$68* (H5)</f>
-        <v>169.5</v>
+        <v>100</v>
       </c>
       <c r="R6" s="23">
         <f t="shared" ref="R6:R7" si="0">R5+I5+L5-K5-M5+0.5* N5+0.5* O5-P6-Q6</f>
-        <v>1360</v>
+        <v>500</v>
       </c>
       <c r="S6" s="17">
         <f>B73</f>
@@ -2226,7 +2277,7 @@
       </c>
       <c r="H7" s="23">
         <f>VLOOKUP($G7,$B$3:$E$6,2,FALSE)</f>
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="I7" s="17">
         <f>VLOOKUP($G7,$B$9:$E$12,2,FALSE)</f>
@@ -2258,15 +2309,15 @@
       </c>
       <c r="P7" s="23">
         <f t="shared" ref="P7" si="1">$B$67/100* (I6+ L6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="23">
         <f>0.01* $B$68* (H6)</f>
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="R7" s="23">
         <f t="shared" si="0"/>
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="S7" s="17">
         <f>B74</f>
@@ -2308,7 +2359,7 @@
       </c>
       <c r="E9" s="17">
         <f>IF(Results!E9= "Eps", 0, Results!E9)</f>
-        <v>10</v>
+        <v>60.000000183920243</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>37</v>
@@ -2322,11 +2373,11 @@
       </c>
       <c r="C10" s="17">
         <f>IF(Results!C10= "Eps", 0, Results!C10)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D10" s="17">
         <f>IF(Results!D10= "Eps", 0, Results!D10)</f>
-        <v>600.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="E10" s="17">
         <f>IF(Results!E10= "Eps", 0, Results!E10)</f>
@@ -2391,7 +2442,7 @@
       </c>
       <c r="E11" s="17">
         <f>IF(Results!E11= "Eps", 0, Results!E11)</f>
-        <v>500.0000000000004</v>
+        <v>500</v>
       </c>
       <c r="G11" s="19">
         <v>0</v>
@@ -2418,19 +2469,19 @@
       </c>
       <c r="M11" s="17">
         <f>F34</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N11" s="17">
         <f>M4</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="O11" s="17">
         <f>D48</f>
-        <v>184</v>
+        <v>26.000000082763837</v>
       </c>
       <c r="P11" s="17">
         <f>E49</f>
-        <v>0</v>
+        <v>2.0000001655280357</v>
       </c>
       <c r="Q11" s="23">
         <v>0</v>
@@ -2474,7 +2525,7 @@
       </c>
       <c r="I12" s="17">
         <f>VLOOKUP($G12,$B$9:$E$12,3,FALSE)</f>
-        <v>600.00000000000011</v>
+        <v>800</v>
       </c>
       <c r="J12" s="17">
         <f>VLOOKUP($G12,$B$15:$E$18,3,FALSE)</f>
@@ -2490,11 +2541,11 @@
       </c>
       <c r="M12" s="17">
         <f>F37</f>
-        <v>10</v>
+        <v>100.00000000000018</v>
       </c>
       <c r="N12" s="17">
         <f t="shared" ref="N12:N14" si="2">M5</f>
-        <v>200</v>
+        <v>130.00000000000017</v>
       </c>
       <c r="O12" s="17">
         <f>D51</f>
@@ -2514,7 +2565,7 @@
       </c>
       <c r="S12" s="17">
         <f>S11+I11+L11-K11+N11-O11+0.5* P11-M11-Q12-R12</f>
-        <v>1400</v>
+        <v>1400.0000000000002</v>
       </c>
       <c r="T12" s="17">
         <f>C72</f>
@@ -2547,11 +2598,11 @@
       </c>
       <c r="M13" s="17">
         <f>F40</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="N13" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>85.000000000000369</v>
       </c>
       <c r="O13" s="17">
         <f>D54</f>
@@ -2563,7 +2614,7 @@
       </c>
       <c r="Q13" s="23">
         <f t="shared" ref="Q13:Q14" si="3">$C$67/100* (I12+ L12)</f>
-        <v>120.00000000000003</v>
+        <v>160</v>
       </c>
       <c r="R13" s="23">
         <f t="shared" ref="R13:R14" si="4">0.01* $C$68* (H12)</f>
@@ -2599,7 +2650,7 @@
       </c>
       <c r="H14" s="17">
         <f>VLOOKUP($G14,$B$3:$E$6,3,FALSE)</f>
-        <v>2540</v>
+        <v>2500</v>
       </c>
       <c r="I14" s="17">
         <f>VLOOKUP($G14,$B$9:$E$12,3,FALSE)</f>
@@ -2643,7 +2694,7 @@
       </c>
       <c r="S14" s="17">
         <f t="shared" si="5"/>
-        <v>2540</v>
+        <v>2500.0000000000005</v>
       </c>
       <c r="T14" s="17">
         <f>C74</f>
@@ -2778,7 +2829,7 @@
       </c>
       <c r="I18" s="23">
         <f>VLOOKUP($G18,$B$9:$E$12,4,FALSE)</f>
-        <v>10</v>
+        <v>60.000000183920243</v>
       </c>
       <c r="J18" s="17">
         <f>VLOOKUP($G18,$B$15:$E$18,4,FALSE)</f>
@@ -2794,15 +2845,15 @@
       </c>
       <c r="M18" s="17">
         <f>M11</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N18" s="17">
         <f>P11</f>
-        <v>0</v>
+        <v>2.0000001655280357</v>
       </c>
       <c r="O18" s="17">
         <f>N4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P18" s="23">
         <v>0</v>
@@ -2841,11 +2892,11 @@
       </c>
       <c r="L19" s="23">
         <f>VLOOKUP($G19,$B$27:$E$30,4,FALSE)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M19" s="17">
         <f t="shared" ref="M19:M21" si="6">M12</f>
-        <v>10</v>
+        <v>100.00000000000018</v>
       </c>
       <c r="N19" s="17">
         <f t="shared" ref="N19:N21" si="7">P12</f>
@@ -2857,7 +2908,7 @@
       </c>
       <c r="P19" s="23">
         <f>$D$67/100* (I18+ L18)</f>
-        <v>1</v>
+        <v>6.0000000183920248</v>
       </c>
       <c r="Q19" s="23">
         <f>0.01* $D$68* (H18)</f>
@@ -2865,7 +2916,7 @@
       </c>
       <c r="R19" s="23">
         <f>R18+I18+L18-K18+M18-N18-O18-P19-Q19</f>
-        <v>1000</v>
+        <v>1000.0000000000002</v>
       </c>
       <c r="S19" s="17">
         <f>D72</f>
@@ -2897,7 +2948,7 @@
       </c>
       <c r="I20" s="23">
         <f>VLOOKUP($G20,$B$9:$E$12,4,FALSE)</f>
-        <v>500.0000000000004</v>
+        <v>500</v>
       </c>
       <c r="J20" s="17">
         <f>VLOOKUP($G20,$B$15:$E$18,4,FALSE)</f>
@@ -2909,11 +2960,11 @@
       </c>
       <c r="L20" s="23">
         <f>VLOOKUP($G20,$B$27:$E$30,4,FALSE)</f>
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="M20" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="N20" s="17">
         <f t="shared" si="7"/>
@@ -2925,7 +2976,7 @@
       </c>
       <c r="P20" s="23">
         <f t="shared" ref="P20:P21" si="9">$D$67/100* (I19+ L19)</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="Q20" s="23">
         <f t="shared" ref="Q20:Q21" si="10">0.01* $D$68* (H19)</f>
@@ -2933,7 +2984,7 @@
       </c>
       <c r="R20" s="23">
         <f t="shared" ref="R20:R21" si="11">R19+I19+L19-K19+M19-N19-O19-P20-Q20</f>
-        <v>1500</v>
+        <v>1500.0000000000005</v>
       </c>
       <c r="S20" s="17">
         <f>D73</f>
@@ -2950,7 +3001,7 @@
       </c>
       <c r="C21" s="17">
         <f>IF(Results!C21= "Eps", 0, Results!C21)</f>
-        <v>0</v>
+        <v>814.0000000413819</v>
       </c>
       <c r="D21" s="17">
         <f>IF(Results!D21= "Eps", 0, Results!D21)</f>
@@ -2965,7 +3016,7 @@
       </c>
       <c r="H21" s="17">
         <f>VLOOKUP($G21,$B$3:$E$6,4,FALSE)</f>
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="I21" s="23">
         <f>VLOOKUP($G21,$B$9:$E$12,4,FALSE)</f>
@@ -2997,7 +3048,7 @@
       </c>
       <c r="P21" s="23">
         <f t="shared" si="9"/>
-        <v>64.000000000000043</v>
+        <v>50</v>
       </c>
       <c r="Q21" s="23">
         <f t="shared" si="10"/>
@@ -3005,7 +3056,7 @@
       </c>
       <c r="R21" s="23">
         <f t="shared" si="11"/>
-        <v>2001.0000000000005</v>
+        <v>2000.0000000000005</v>
       </c>
       <c r="S21" s="17">
         <f>D74</f>
@@ -3020,7 +3071,7 @@
       </c>
       <c r="C22" s="17">
         <f>IF(Results!C22= "Eps", 0, Results!C22)</f>
-        <v>0</v>
+        <v>269.99999999999983</v>
       </c>
       <c r="D22" s="17">
         <f>IF(Results!D22= "Eps", 0, Results!D22)</f>
@@ -3039,7 +3090,7 @@
       </c>
       <c r="C23" s="17">
         <f>IF(Results!C23= "Eps", 0, Results!C23)</f>
-        <v>0</v>
+        <v>364.99999999999966</v>
       </c>
       <c r="D23" s="17">
         <f>IF(Results!D23= "Eps", 0, Results!D23)</f>
@@ -3073,7 +3124,7 @@
       </c>
       <c r="H24" s="21">
         <f>Results!B65</f>
-        <v>400</v>
+        <v>198500.00000000029</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -3106,7 +3157,7 @@
       </c>
       <c r="H26" s="21">
         <f>Results!B69</f>
-        <v>0</v>
+        <v>289800.00000827626</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -3119,7 +3170,7 @@
       </c>
       <c r="C27" s="17">
         <f>IF(Results!C27= "Eps", 0, Results!C27)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D27" s="17">
         <f>IF(Results!D27= "Eps", 0, Results!D27)</f>
@@ -3134,7 +3185,7 @@
       </c>
       <c r="H27" s="21">
         <f>Results!B71</f>
-        <v>738000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -3153,14 +3204,14 @@
       </c>
       <c r="E28" s="17">
         <f>IF(Results!E28= "Eps", 0, Results!E28)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="21">
         <f>Results!B73</f>
-        <v>738400</v>
+        <v>488300.00000827655</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -3171,7 +3222,7 @@
       </c>
       <c r="C29" s="17">
         <f>IF(Results!C29= "Eps", 0, Results!C29)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D29" s="17">
         <f>IF(Results!D29= "Eps", 0, Results!D29)</f>
@@ -3179,7 +3230,7 @@
       </c>
       <c r="E29" s="17">
         <f>IF(Results!E29= "Eps", 0, Results!E29)</f>
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -3235,7 +3286,7 @@
       </c>
       <c r="E33" s="17">
         <f>IF(Results!E33= "Eps", 0, Results!E33)</f>
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3250,7 +3301,7 @@
       </c>
       <c r="F34" s="17">
         <f>IF(Results!F34= "Eps", 0, Results!F34)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3276,7 +3327,7 @@
       </c>
       <c r="E36" s="17">
         <f>IF(Results!E36= "Eps", 0, Results!E36)</f>
-        <v>200</v>
+        <v>130.00000000000017</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3291,7 +3342,7 @@
       </c>
       <c r="F37" s="17">
         <f>IF(Results!F37= "Eps", 0, Results!F37)</f>
-        <v>10</v>
+        <v>100.00000000000018</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3317,7 +3368,7 @@
       </c>
       <c r="E39" s="17">
         <f>IF(Results!E39= "Eps", 0, Results!E39)</f>
-        <v>0</v>
+        <v>85.000000000000369</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -3332,7 +3383,7 @@
       </c>
       <c r="F40" s="17">
         <f>IF(Results!F40= "Eps", 0, Results!F40)</f>
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3429,7 +3480,7 @@
       </c>
       <c r="D48" s="17">
         <f>IF(Results!D52= "Eps", 0, Results!D52)</f>
-        <v>184</v>
+        <v>26.000000082763837</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -3444,11 +3495,11 @@
       </c>
       <c r="D49" s="17">
         <f>IF(Results!D53= "Eps", 0, Results!D53)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E49" s="17">
         <f>IF(Results!E53= "Eps", 0, Results!E53)</f>
-        <v>0</v>
+        <v>2.0000001655280357</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
end of phase 2
</commit_message>
<xml_diff>
--- a/Phase2-answer/Pahse2_Data_OR2.xlsx
+++ b/Phase2-answer/Pahse2_Data_OR2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase2-answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6368B9-44B4-4621-A5B2-05508DF3DB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F486CEE9-D27E-4F71-82AF-0A809055F18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="11" xr2:uid="{ECF2C842-86F1-4BFD-957D-54F5363C8BBA}"/>
   </bookViews>
@@ -266,7 +266,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -551,8 +551,8 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1AFE74-D632-48D7-84D6-FBBFA6DF1ECB}">
   <dimension ref="A2:T74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2457,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D915A85-1C44-4365-B131-3DC9A2FE90C9}">
   <dimension ref="A2:T74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3941,7 +3941,7 @@
   <dimension ref="C2:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>